<commit_message>
excel dateien und csv
</commit_message>
<xml_diff>
--- a/Immos/nebenkostenabrechung.xlsx
+++ b/Immos/nebenkostenabrechung.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="151">
   <si>
     <t>briefDatum</t>
   </si>
@@ -64,7 +64,7 @@
     <t>mitKonto</t>
   </si>
   <si>
-    <t>09.06.15</t>
+    <t>01.07.15</t>
   </si>
   <si>
     <t>Familie</t>
@@ -88,229 +88,271 @@
     <t>2014</t>
   </si>
   <si>
-    <t>0</t>
+    <t>-414,23</t>
+  </si>
+  <si>
+    <t>0002627370</t>
+  </si>
+  <si>
+    <t>44350060</t>
+  </si>
+  <si>
+    <t>Kreis- und Stadtsparkasse Unna,59409 Unna</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>Mischke</t>
+  </si>
+  <si>
+    <t>-170,29</t>
+  </si>
+  <si>
+    <t>2202770602</t>
+  </si>
+  <si>
+    <t>44160014</t>
+  </si>
+  <si>
+    <t>Dortmunder Volksbank,44128 Dortmund</t>
+  </si>
+  <si>
+    <t>Herr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Werner Hessel </t>
+  </si>
+  <si>
+    <t>Sehr geehrter Herr</t>
+  </si>
+  <si>
+    <t>Hessel</t>
+  </si>
+  <si>
+    <t>-99,77</t>
+  </si>
+  <si>
+    <t>2203298601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herr  Werner Hessel </t>
+  </si>
+  <si>
+    <t>Frau</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Christine Krämer-Kersting </t>
+  </si>
+  <si>
+    <t>Sehr geehrte Frau</t>
+  </si>
+  <si>
+    <t>Krämer-Kersting</t>
+  </si>
+  <si>
+    <t>-249,76</t>
+  </si>
+  <si>
+    <t>2420350701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frau  Christine Krämer-Kersting </t>
+  </si>
+  <si>
+    <t>Haine-Maida</t>
+  </si>
+  <si>
+    <t>-253,19</t>
+  </si>
+  <si>
+    <t>0003628658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betriebskostenabrechnung </t>
+  </si>
+  <si>
+    <t>Monat:01-12</t>
+  </si>
+  <si>
+    <t>Saarbrückerweg  24 , 59439  Holzwickede,2014,vom:17.05.15</t>
+  </si>
+  <si>
+    <t>Mieter:</t>
+  </si>
+  <si>
+    <t>Kostenart</t>
+  </si>
+  <si>
+    <t>UmlSchl</t>
+  </si>
+  <si>
+    <t>Ges €</t>
+  </si>
+  <si>
+    <t>x (Anteil</t>
+  </si>
+  <si>
+    <t>/ MengeGes) =</t>
+  </si>
+  <si>
+    <t>€</t>
+  </si>
+  <si>
+    <t>Entwässerung</t>
+  </si>
+  <si>
+    <t>Zaehler cbm</t>
+  </si>
+  <si>
+    <t>1.104,00</t>
+  </si>
+  <si>
+    <t>12,080+26,640+65,803</t>
+  </si>
+  <si>
+    <t>317,767</t>
+  </si>
+  <si>
+    <t>363,14</t>
+  </si>
+  <si>
+    <t>Entwässerung Fläche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qm </t>
+  </si>
+  <si>
+    <t>263,94</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>386</t>
+  </si>
+  <si>
+    <t>76,58</t>
+  </si>
+  <si>
+    <t>Grundsteuer</t>
+  </si>
+  <si>
+    <t>1.126,38</t>
+  </si>
+  <si>
+    <t>326,83</t>
+  </si>
+  <si>
+    <t>Müllabfuhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personen </t>
+  </si>
+  <si>
+    <t>794,64</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>317,86</t>
+  </si>
+  <si>
+    <t>Müllabfuhr Bio</t>
+  </si>
+  <si>
+    <t>107,52</t>
+  </si>
+  <si>
+    <t>43,01</t>
+  </si>
+  <si>
+    <t>Gebäudeversicherung</t>
+  </si>
+  <si>
+    <t>753,86</t>
+  </si>
+  <si>
+    <t>218,74</t>
+  </si>
+  <si>
+    <t>Grundstückspflege</t>
+  </si>
+  <si>
+    <t>748,51</t>
+  </si>
+  <si>
+    <t>217,18</t>
+  </si>
+  <si>
+    <t>Haftpflichtversicherung</t>
+  </si>
+  <si>
+    <t>115,00</t>
+  </si>
+  <si>
+    <t>33,37</t>
+  </si>
+  <si>
+    <t>Kabelfernsehen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haushalt </t>
+  </si>
+  <si>
+    <t>991,20</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>198,24</t>
+  </si>
+  <si>
+    <t>Mietwasseruhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stck </t>
+  </si>
+  <si>
+    <t>189,20</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>51,60</t>
+  </si>
+  <si>
+    <t>Wasser</t>
+  </si>
+  <si>
+    <t>753,00</t>
+  </si>
+  <si>
+    <t>247,68</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>nein</t>
-  </si>
-  <si>
-    <t>Mischke</t>
-  </si>
-  <si>
-    <t>Hessel</t>
-  </si>
-  <si>
-    <t>2203298601</t>
-  </si>
-  <si>
-    <t>44160014</t>
-  </si>
-  <si>
-    <t>Dortmunder Volksbank,44128 Dortmund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herr  Werner Hessel </t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
-    <t>Krämer-Kersting</t>
-  </si>
-  <si>
-    <t>2420350701</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frau  Christine Krämer-Kersting </t>
-  </si>
-  <si>
-    <t>Haine-Maida</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Betriebskostenabrechnung </t>
-  </si>
-  <si>
-    <t>Monat:01-12</t>
-  </si>
-  <si>
-    <t>Saarbrückerweg  24 , 59439  Holzwickede,2014,vom:17.05.15</t>
-  </si>
-  <si>
-    <t>Mieter:</t>
-  </si>
-  <si>
-    <t>Kostenart</t>
-  </si>
-  <si>
-    <t>UmlSchl</t>
-  </si>
-  <si>
-    <t>Ges €</t>
-  </si>
-  <si>
-    <t>x (Anteil</t>
-  </si>
-  <si>
-    <t>/ MengeGes) =</t>
-  </si>
-  <si>
-    <t>€</t>
-  </si>
-  <si>
-    <t>Entwässerung</t>
-  </si>
-  <si>
-    <t>Zaehler cbm</t>
-  </si>
-  <si>
-    <t>1.104,00</t>
-  </si>
-  <si>
-    <t>65,803+26,640+12,080</t>
-  </si>
-  <si>
-    <t>317,767</t>
-  </si>
-  <si>
-    <t>363,14</t>
-  </si>
-  <si>
-    <t>Entwässerung Fläche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qm </t>
-  </si>
-  <si>
-    <t>263,94</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>386</t>
-  </si>
-  <si>
-    <t>76,58</t>
-  </si>
-  <si>
-    <t>Grundsteuer</t>
-  </si>
-  <si>
-    <t>1.126,38</t>
-  </si>
-  <si>
-    <t>326,83</t>
-  </si>
-  <si>
-    <t>Müllabfuhr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personen </t>
-  </si>
-  <si>
-    <t>794,64</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>317,86</t>
-  </si>
-  <si>
-    <t>Müllabfuhr Bio</t>
-  </si>
-  <si>
-    <t>107,52</t>
-  </si>
-  <si>
-    <t>43,01</t>
-  </si>
-  <si>
-    <t>Gebäudeversicherung</t>
-  </si>
-  <si>
-    <t>753,86</t>
-  </si>
-  <si>
-    <t>218,74</t>
-  </si>
-  <si>
-    <t>Grundstückspflege</t>
-  </si>
-  <si>
-    <t>748,51</t>
-  </si>
-  <si>
-    <t>217,18</t>
-  </si>
-  <si>
-    <t>Haftpflichtversicherung</t>
-  </si>
-  <si>
-    <t>115,00</t>
-  </si>
-  <si>
-    <t>33,37</t>
-  </si>
-  <si>
-    <t>Kabelfernsehen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haushalt </t>
-  </si>
-  <si>
-    <t>991,20</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>198,24</t>
-  </si>
-  <si>
-    <t>Mietwasseruhr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stck </t>
-  </si>
-  <si>
-    <t>189,20</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>51,60</t>
-  </si>
-  <si>
-    <t>Wasser</t>
-  </si>
-  <si>
-    <t>753,00</t>
-  </si>
-  <si>
-    <t>247,68</t>
-  </si>
-  <si>
     <t>Summe</t>
   </si>
   <si>
     <t>2.094,23</t>
   </si>
   <si>
-    <t>13,590+49,672</t>
+    <t>49,672+13,590</t>
   </si>
   <si>
     <t>219,79</t>
@@ -352,7 +394,7 @@
     <t>1.250,29</t>
   </si>
   <si>
-    <t>5,845+29,988</t>
+    <t>29,988+5,845</t>
   </si>
   <si>
     <t>124,49</t>
@@ -370,7 +412,7 @@
     <t>999,77</t>
   </si>
   <si>
-    <t>32,585+11,047</t>
+    <t>11,047+32,585</t>
   </si>
   <si>
     <t>151,59</t>
@@ -563,16 +605,16 @@
         <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
@@ -583,7 +625,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -595,7 +637,7 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
@@ -604,22 +646,22 @@
         <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="N3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -627,10 +669,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>18</v>
@@ -639,10 +681,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
@@ -651,22 +693,22 @@
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="O4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -674,10 +716,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -686,10 +728,10 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
@@ -698,22 +740,22 @@
         <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N5" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="O5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -724,7 +766,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -736,7 +778,7 @@
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>
@@ -745,22 +787,22 @@
         <v>22</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N6" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="O6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -786,23 +828,23 @@
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" ht="21.0" customHeight="true">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="true">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -810,262 +852,262 @@
     </row>
     <row r="4" ht="21.0" customHeight="true">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="true">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="true">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="true">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="true">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="true">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="true">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="true">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="true">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="true">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="true">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="true">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="true">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1091,286 +1133,286 @@
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" ht="21.0" customHeight="true">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="true">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="true">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="true">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="true">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="true">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="true">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="true">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="true">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="true">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="true">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="true">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="true">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="true">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="true">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1396,286 +1438,286 @@
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" ht="21.0" customHeight="true">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="true">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="true">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="true">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="true">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="true">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="true">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="true">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="true">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="true">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="true">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="true">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="true">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="true">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="true">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1701,286 +1743,286 @@
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" ht="21.0" customHeight="true">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="true">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="true">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="true">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="true">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="true">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="true">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="true">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="true">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="true">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="true">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="true">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="true">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="true">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="true">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2006,286 +2048,286 @@
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" ht="21.0" customHeight="true">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" ht="21.0" customHeight="true">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" ht="21.0" customHeight="true">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" ht="21.0" customHeight="true">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" ht="21.0" customHeight="true">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" ht="21.0" customHeight="true">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" ht="21.0" customHeight="true">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" ht="21.0" customHeight="true">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" ht="21.0" customHeight="true">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" ht="21.0" customHeight="true">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" ht="21.0" customHeight="true">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" ht="21.0" customHeight="true">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" ht="21.0" customHeight="true">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" ht="21.0" customHeight="true">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" ht="21.0" customHeight="true">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Querformat Excel Ausgabe, landscape(true)
</commit_message>
<xml_diff>
--- a/Immos/nebenkostenabrechung.xlsx
+++ b/Immos/nebenkostenabrechung.xlsx
@@ -64,7 +64,7 @@
     <t>mitKonto</t>
   </si>
   <si>
-    <t>03.07.15</t>
+    <t>04.07.15</t>
   </si>
   <si>
     <t>Familie</t>
@@ -995,18 +995,18 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="21.484375" customWidth="true"/>
-    <col min="2" max="2" width="15.625" customWidth="true"/>
-    <col min="3" max="3" width="15.625" customWidth="true"/>
-    <col min="4" max="4" width="15.625" customWidth="true"/>
-    <col min="5" max="5" width="15.625" customWidth="true"/>
-    <col min="6" max="6" width="15.625" customWidth="true"/>
+    <col min="2" max="2" width="13.671875" customWidth="true"/>
+    <col min="3" max="3" width="13.671875" customWidth="true"/>
+    <col min="4" max="4" width="13.671875" customWidth="true"/>
+    <col min="5" max="5" width="13.671875" customWidth="true"/>
+    <col min="6" max="6" width="13.671875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1022,7 +1022,7 @@
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
       <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1050,7 +1050,7 @@
       <c r="A5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1070,7 +1070,7 @@
       <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1090,7 +1090,7 @@
       <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1110,7 +1110,7 @@
       <c r="A8" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1130,7 +1130,7 @@
       <c r="A9" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1150,7 +1150,7 @@
       <c r="A10" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1170,7 +1170,7 @@
       <c r="A11" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1190,7 +1190,7 @@
       <c r="A12" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1210,7 +1210,7 @@
       <c r="A13" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1230,7 +1230,7 @@
       <c r="A14" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1250,7 +1250,7 @@
       <c r="A15" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1270,7 +1270,7 @@
       <c r="A16" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1291,7 +1291,7 @@
       <c r="A18" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>112</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1305,7 +1305,7 @@
       <c r="A19" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>116</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1319,7 +1319,7 @@
       <c r="A20" t="s">
         <v>119</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>120</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1333,7 +1333,7 @@
       <c r="A21" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>124</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1347,7 +1347,7 @@
       <c r="A22" t="s">
         <v>127</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>128</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1361,7 +1361,7 @@
       <c r="A23" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>108</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1373,6 +1373,7 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
 </worksheet>
 </file>
 
@@ -1385,18 +1386,18 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="21.484375" customWidth="true"/>
-    <col min="2" max="2" width="15.625" customWidth="true"/>
-    <col min="3" max="3" width="15.625" customWidth="true"/>
-    <col min="4" max="4" width="15.625" customWidth="true"/>
-    <col min="5" max="5" width="15.625" customWidth="true"/>
-    <col min="6" max="6" width="15.625" customWidth="true"/>
+    <col min="2" max="2" width="13.671875" customWidth="true"/>
+    <col min="3" max="3" width="13.671875" customWidth="true"/>
+    <col min="4" max="4" width="13.671875" customWidth="true"/>
+    <col min="5" max="5" width="13.671875" customWidth="true"/>
+    <col min="6" max="6" width="13.671875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1412,7 +1413,7 @@
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1420,7 +1421,7 @@
       <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1440,7 +1441,7 @@
       <c r="A5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1460,7 +1461,7 @@
       <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1480,7 +1481,7 @@
       <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1500,7 +1501,7 @@
       <c r="A8" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1520,7 +1521,7 @@
       <c r="A9" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1540,7 +1541,7 @@
       <c r="A10" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1560,7 +1561,7 @@
       <c r="A11" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1580,7 +1581,7 @@
       <c r="A12" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1600,7 +1601,7 @@
       <c r="A13" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1620,7 +1621,7 @@
       <c r="A14" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1640,7 +1641,7 @@
       <c r="A15" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1660,7 +1661,7 @@
       <c r="A16" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1681,7 +1682,7 @@
       <c r="A18" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>112</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1695,7 +1696,7 @@
       <c r="A19" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>146</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1709,7 +1710,7 @@
       <c r="A20" t="s">
         <v>149</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>150</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1723,7 +1724,7 @@
       <c r="A21" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>108</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1735,6 +1736,7 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
 </worksheet>
 </file>
 
@@ -1747,18 +1749,18 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="21.484375" customWidth="true"/>
-    <col min="2" max="2" width="15.625" customWidth="true"/>
-    <col min="3" max="3" width="15.625" customWidth="true"/>
-    <col min="4" max="4" width="15.625" customWidth="true"/>
-    <col min="5" max="5" width="15.625" customWidth="true"/>
-    <col min="6" max="6" width="15.625" customWidth="true"/>
+    <col min="2" max="2" width="13.671875" customWidth="true"/>
+    <col min="3" max="3" width="13.671875" customWidth="true"/>
+    <col min="4" max="4" width="13.671875" customWidth="true"/>
+    <col min="5" max="5" width="13.671875" customWidth="true"/>
+    <col min="6" max="6" width="13.671875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1774,7 +1776,7 @@
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1782,7 +1784,7 @@
       <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1802,7 +1804,7 @@
       <c r="A5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1822,7 +1824,7 @@
       <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1842,7 +1844,7 @@
       <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1862,7 +1864,7 @@
       <c r="A8" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1882,7 +1884,7 @@
       <c r="A9" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1902,7 +1904,7 @@
       <c r="A10" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1922,7 +1924,7 @@
       <c r="A11" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1942,7 +1944,7 @@
       <c r="A12" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1962,7 +1964,7 @@
       <c r="A13" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1982,7 +1984,7 @@
       <c r="A14" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2002,7 +2004,7 @@
       <c r="A15" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2022,7 +2024,7 @@
       <c r="A16" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2043,7 +2045,7 @@
       <c r="A18" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>112</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2057,7 +2059,7 @@
       <c r="A19" t="s">
         <v>160</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>161</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2071,7 +2073,7 @@
       <c r="A20" t="s">
         <v>164</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>165</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2085,7 +2087,7 @@
       <c r="A21" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>108</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -2097,6 +2099,7 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
 </worksheet>
 </file>
 
@@ -2109,18 +2112,18 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="21.484375" customWidth="true"/>
-    <col min="2" max="2" width="15.625" customWidth="true"/>
-    <col min="3" max="3" width="15.625" customWidth="true"/>
-    <col min="4" max="4" width="15.625" customWidth="true"/>
-    <col min="5" max="5" width="15.625" customWidth="true"/>
-    <col min="6" max="6" width="15.625" customWidth="true"/>
+    <col min="2" max="2" width="13.671875" customWidth="true"/>
+    <col min="3" max="3" width="13.671875" customWidth="true"/>
+    <col min="4" max="4" width="13.671875" customWidth="true"/>
+    <col min="5" max="5" width="13.671875" customWidth="true"/>
+    <col min="6" max="6" width="13.671875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2136,7 +2139,7 @@
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2144,7 +2147,7 @@
       <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2164,7 +2167,7 @@
       <c r="A5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2184,7 +2187,7 @@
       <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2204,7 +2207,7 @@
       <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2224,7 +2227,7 @@
       <c r="A8" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2244,7 +2247,7 @@
       <c r="A9" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2264,7 +2267,7 @@
       <c r="A10" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2284,7 +2287,7 @@
       <c r="A11" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2304,7 +2307,7 @@
       <c r="A12" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2324,7 +2327,7 @@
       <c r="A13" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2344,7 +2347,7 @@
       <c r="A14" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2364,7 +2367,7 @@
       <c r="A15" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2384,7 +2387,7 @@
       <c r="A16" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2405,7 +2408,7 @@
       <c r="A18" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>112</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2419,7 +2422,7 @@
       <c r="A19" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>180</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2433,7 +2436,7 @@
       <c r="A20" t="s">
         <v>183</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>184</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2447,7 +2450,7 @@
       <c r="A21" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>108</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -2459,6 +2462,7 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
 </worksheet>
 </file>
 
@@ -2471,18 +2475,18 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="21.484375" customWidth="true"/>
-    <col min="2" max="2" width="15.625" customWidth="true"/>
-    <col min="3" max="3" width="15.625" customWidth="true"/>
-    <col min="4" max="4" width="15.625" customWidth="true"/>
-    <col min="5" max="5" width="15.625" customWidth="true"/>
-    <col min="6" max="6" width="15.625" customWidth="true"/>
+    <col min="2" max="2" width="13.671875" customWidth="true"/>
+    <col min="3" max="3" width="13.671875" customWidth="true"/>
+    <col min="4" max="4" width="13.671875" customWidth="true"/>
+    <col min="5" max="5" width="13.671875" customWidth="true"/>
+    <col min="6" max="6" width="13.671875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.0" customHeight="true">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2498,7 +2502,7 @@
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2506,7 +2510,7 @@
       <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2526,7 +2530,7 @@
       <c r="A5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2546,7 +2550,7 @@
       <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2566,7 +2570,7 @@
       <c r="A7" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2586,7 +2590,7 @@
       <c r="A8" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2606,7 +2610,7 @@
       <c r="A9" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>76</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2626,7 +2630,7 @@
       <c r="A10" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2646,7 +2650,7 @@
       <c r="A11" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2666,7 +2670,7 @@
       <c r="A12" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2686,7 +2690,7 @@
       <c r="A13" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2706,7 +2710,7 @@
       <c r="A14" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2726,7 +2730,7 @@
       <c r="A15" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2746,7 +2750,7 @@
       <c r="A16" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2767,7 +2771,7 @@
       <c r="A18" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>112</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2781,7 +2785,7 @@
       <c r="A19" t="s">
         <v>198</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>199</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2795,7 +2799,7 @@
       <c r="A20" t="s">
         <v>202</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>203</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2809,7 +2813,7 @@
       <c r="A21" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>108</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -2821,5 +2825,6 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Abrechnungsbriefe wieder in DruckController
</commit_message>
<xml_diff>
--- a/Immos/nebenkostenabrechung.xlsx
+++ b/Immos/nebenkostenabrechung.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Diener" r:id="rId3" sheetId="1"/>
+    <sheet name="Brzoza" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -23,13 +23,13 @@
     <t>Monat:01-12</t>
   </si>
   <si>
-    <t>Haferkamp  1 , 59192  Bergkamen,Doppelhaushälfte,li,EG,DG</t>
+    <t>Haferkamp  3 , 59192  Bergkamen,Doppelhaushälfte,re,EG,DG</t>
   </si>
   <si>
     <t>Mieter:</t>
   </si>
   <si>
-    <t>Diener</t>
+    <t>Brzoza</t>
   </si>
   <si>
     <t>Kostenart</t>
@@ -50,22 +50,22 @@
     <t>€</t>
   </si>
   <si>
-    <t>Entwässerung</t>
+    <t>Entwässerung Fläche</t>
   </si>
   <si>
     <t xml:space="preserve">Haushalt </t>
   </si>
   <si>
-    <t>608,82</t>
+    <t>168,96</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>Entwässerung Fläche</t>
-  </si>
-  <si>
-    <t>168,96</t>
+    <t>Entwässerung Verbrauch</t>
+  </si>
+  <si>
+    <t>784,02</t>
   </si>
   <si>
     <t>Grundsteuer</t>
@@ -77,7 +77,7 @@
     <t>Müllabfuhr</t>
   </si>
   <si>
-    <t>236,40</t>
+    <t>118,20</t>
   </si>
   <si>
     <t>Müllabfuhr Bio</t>
@@ -101,7 +101,7 @@
     <t>Heizungswartung</t>
   </si>
   <si>
-    <t>122,68</t>
+    <t>121,46</t>
   </si>
   <si>
     <t>Rauchmelder</t>
@@ -116,7 +116,7 @@
     <t>Summe</t>
   </si>
   <si>
-    <t>1.863,69</t>
+    <t>1.919,47</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Aufbereitung Valutadatum beim Druck der Zahlungszuordnung
</commit_message>
<xml_diff>
--- a/Immos/nebenkostenabrechung.xlsx
+++ b/Immos/nebenkostenabrechung.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Brzoza" r:id="rId3" sheetId="1"/>
+    <sheet name="Partu" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -23,13 +23,13 @@
     <t>Monat:01-12</t>
   </si>
   <si>
-    <t>Haferkamp  3 , 59192  Bergkamen,Doppelhaushälfte,re,EG,DG</t>
+    <t>Heinrichstraße  46 , 59077  Hamm,Reihenmittelhaus,</t>
   </si>
   <si>
     <t>Mieter:</t>
   </si>
   <si>
-    <t>Brzoza</t>
+    <t>Partu</t>
   </si>
   <si>
     <t>Kostenart</t>
@@ -50,64 +50,64 @@
     <t>€</t>
   </si>
   <si>
-    <t>Entwässerung Fläche</t>
+    <t>Entwässerung</t>
   </si>
   <si>
     <t xml:space="preserve">Haushalt </t>
   </si>
   <si>
-    <t>168,96</t>
+    <t>84,00</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>Entwässerung Verbrauch</t>
-  </si>
-  <si>
-    <t>784,02</t>
-  </si>
-  <si>
     <t>Grundsteuer</t>
   </si>
   <si>
-    <t>318,85</t>
+    <t>301,50</t>
   </si>
   <si>
     <t>Müllabfuhr</t>
   </si>
   <si>
-    <t>118,20</t>
-  </si>
-  <si>
-    <t>Müllabfuhr Bio</t>
-  </si>
-  <si>
-    <t>53,70</t>
+    <t>147,62</t>
   </si>
   <si>
     <t>Gebäudeversicherung</t>
   </si>
   <si>
-    <t>280,00</t>
+    <t>231,95</t>
   </si>
   <si>
     <t>Haftpflichtversicherung</t>
   </si>
   <si>
-    <t>43,91</t>
+    <t>46,10</t>
   </si>
   <si>
     <t>Heizungswartung</t>
   </si>
   <si>
-    <t>121,46</t>
+    <t>163,60</t>
+  </si>
+  <si>
+    <t>Kabelfernsehen</t>
+  </si>
+  <si>
+    <t>146,28</t>
   </si>
   <si>
     <t>Rauchmelder</t>
   </si>
   <si>
-    <t>30,37</t>
+    <t>111,45</t>
+  </si>
+  <si>
+    <t>Schornsteinfeger</t>
+  </si>
+  <si>
+    <t>64,55</t>
   </si>
   <si>
     <t/>
@@ -116,7 +116,7 @@
     <t>Summe</t>
   </si>
   <si>
-    <t>1.919,47</t>
+    <t>1.297,05</t>
   </si>
 </sst>
 </file>

</xml_diff>